<commit_message>
Update: -export pdf dan excel pada laporan tagihan, -format contoh format import excel transaksi pembayaran
</commit_message>
<xml_diff>
--- a/public/template/contoh_format_pembayaran.xlsx
+++ b/public/template/contoh_format_pembayaran.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>settlement</t>
   </si>
@@ -32,9 +32,6 @@
     <t>loket</t>
   </si>
   <si>
-    <t>juli</t>
-  </si>
-  <si>
     <t>8257062100000000</t>
   </si>
   <si>
@@ -59,10 +56,25 @@
     <t>Dibayar</t>
   </si>
   <si>
-    <t>Bajragin Thamrin</t>
-  </si>
-  <si>
-    <t>per siswa Bajragin Thamrin</t>
+    <t>Tahun Ajaran</t>
+  </si>
+  <si>
+    <t>2020/2021</t>
+  </si>
+  <si>
+    <t>Mila Kusmawati</t>
+  </si>
+  <si>
+    <t>spp</t>
+  </si>
+  <si>
+    <t>bebas</t>
+  </si>
+  <si>
+    <t>8257062100000022</t>
+  </si>
+  <si>
+    <t>2021/2022</t>
   </si>
 </sst>
 </file>
@@ -396,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,35 +427,38 @@
     <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -452,18 +467,43 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>110000</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3">
         <v>90000</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="D3" s="2"/>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Menghapus No VA PMB pada import transaksi pembayaran
</commit_message>
<xml_diff>
--- a/public/template/contoh_format_pembayaran.xlsx
+++ b/public/template/contoh_format_pembayaran.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\807zu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Laravel\New folder\spp\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>settlement</t>
   </si>
@@ -32,15 +32,9 @@
     <t>loket</t>
   </si>
   <si>
-    <t>8257062100000000</t>
-  </si>
-  <si>
     <t>Nama Siswa</t>
   </si>
   <si>
-    <t>No VA PMB</t>
-  </si>
-  <si>
     <t>Metode Pembayaran</t>
   </si>
   <si>
@@ -62,19 +56,16 @@
     <t>2020/2021</t>
   </si>
   <si>
-    <t>Mila Kusmawati</t>
-  </si>
-  <si>
-    <t>spp</t>
-  </si>
-  <si>
-    <t>bebas</t>
-  </si>
-  <si>
-    <t>8257062100000022</t>
-  </si>
-  <si>
-    <t>2021/2022</t>
+    <t>Paramita Wahyuni</t>
+  </si>
+  <si>
+    <t>SPP 1</t>
+  </si>
+  <si>
+    <t>Juli</t>
+  </si>
+  <si>
+    <t>Agustus</t>
   </si>
 </sst>
 </file>
@@ -123,9 +114,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -408,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G3" sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,90 +409,81 @@
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>125000</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2">
-        <v>110000</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="D3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <v>90000</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
+      <c r="F3">
+        <v>100000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
validasi import siswa & pembayaran, menampilkan kembali no VA PMB
</commit_message>
<xml_diff>
--- a/public/template/contoh_format_pembayaran.xlsx
+++ b/public/template/contoh_format_pembayaran.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Laravel\New folder\spp\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\807zu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>settlement</t>
   </si>
@@ -66,13 +66,22 @@
   </si>
   <si>
     <t>Agustus</t>
+  </si>
+  <si>
+    <t>No VA PMB</t>
+  </si>
+  <si>
+    <t>8257062100000000</t>
+  </si>
+  <si>
+    <t>8257062100000022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +98,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,10 +131,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="A1:G3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,72 +437,81 @@
     <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>125000</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>100000</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tanggal transaksi berdasarkan tgl import pembayaran dan update laporan pdf(total)
</commit_message>
<xml_diff>
--- a/public/template/contoh_format_pembayaran.xlsx
+++ b/public/template/contoh_format_pembayaran.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>settlement</t>
   </si>
@@ -56,18 +56,6 @@
     <t>2020/2021</t>
   </si>
   <si>
-    <t>Paramita Wahyuni</t>
-  </si>
-  <si>
-    <t>SPP 1</t>
-  </si>
-  <si>
-    <t>Juli</t>
-  </si>
-  <si>
-    <t>Agustus</t>
-  </si>
-  <si>
     <t>No VA PMB</t>
   </si>
   <si>
@@ -75,6 +63,21 @@
   </si>
   <si>
     <t>8257062100000022</t>
+  </si>
+  <si>
+    <t>Tanggal Bayar</t>
+  </si>
+  <si>
+    <t>Anastasia Novitasari</t>
+  </si>
+  <si>
+    <t>SPP1</t>
+  </si>
+  <si>
+    <t>Januari</t>
+  </si>
+  <si>
+    <t>Februari</t>
   </si>
 </sst>
 </file>
@@ -131,13 +134,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,12 +438,13 @@
     <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -462,13 +467,16 @@
       <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -477,10 +485,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G2">
         <v>125000</v>
@@ -488,13 +496,16 @@
       <c r="H2" t="s">
         <v>9</v>
       </c>
+      <c r="I2" s="6">
+        <v>44359.396527777775</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -503,16 +514,19 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G3">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="H3" t="s">
         <v>9</v>
+      </c>
+      <c r="I3" s="6">
+        <v>44360.638888888891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update sebelum masuk ke jenis pembayaran dan import data
</commit_message>
<xml_diff>
--- a/public/template/contoh_format_pembayaran.xlsx
+++ b/public/template/contoh_format_pembayaran.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\807zu\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,29 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
-  <si>
-    <t>settlement</t>
-  </si>
-  <si>
-    <t>loket</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Nama Siswa</t>
   </si>
   <si>
-    <t>Metode Pembayaran</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Nama Pembayaran</t>
-  </si>
-  <si>
-    <t>Keterangan</t>
-  </si>
-  <si>
     <t>Dibayar</t>
   </si>
   <si>
@@ -56,44 +33,26 @@
     <t>2020/2021</t>
   </si>
   <si>
-    <t>No VA PMB</t>
-  </si>
-  <si>
-    <t>8257062100000000</t>
-  </si>
-  <si>
-    <t>8257062100000022</t>
-  </si>
-  <si>
     <t>Tanggal Bayar</t>
   </si>
   <si>
-    <t>Anastasia Novitasari</t>
-  </si>
-  <si>
-    <t>SPP1</t>
-  </si>
-  <si>
-    <t>Januari</t>
-  </si>
-  <si>
-    <t>Februari</t>
+    <t>semester</t>
+  </si>
+  <si>
+    <t>Paiman Kuswoyo</t>
+  </si>
+  <si>
+    <t>no_va_pmb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,24 +64,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -130,18 +87,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -202,7 +180,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -237,7 +215,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -414,7 +392,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -422,111 +400,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>8257062100000000</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3">
+        <v>30000</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2">
-        <v>125000</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="6">
+      <c r="F2" s="4">
         <v>44359.396527777775</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3">
-        <v>50000</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="6">
-        <v>44360.638888888891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>